<commit_message>
#Added deer as separate spp. for bsl data #Made final graphs and tables
</commit_message>
<xml_diff>
--- a/data/rai and boots results - both camps.xlsx
+++ b/data/rai and boots results - both camps.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="31">
   <si>
     <t>name_sci</t>
   </si>
@@ -103,6 +103,15 @@
   </si>
   <si>
     <t>Camp 2</t>
+  </si>
+  <si>
+    <t>rai_round</t>
+  </si>
+  <si>
+    <t>Run2</t>
+  </si>
+  <si>
+    <t>Run3</t>
   </si>
 </sst>
 </file>
@@ -909,20 +918,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:V36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="0" hidden="1" customWidth="1"/>
+    <col min="6" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="18" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="0" hidden="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="S1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -941,8 +965,50 @@
       <c r="F2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M2" t="s">
+        <v>5</v>
+      </c>
+      <c r="N2" t="s">
+        <v>28</v>
+      </c>
+      <c r="P2" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>2</v>
+      </c>
+      <c r="S2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T2" t="s">
+        <v>4</v>
+      </c>
+      <c r="U2" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -961,8 +1027,50 @@
       <c r="F3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0.382653061224489</v>
+      </c>
+      <c r="K3">
+        <v>0.12653061224489701</v>
+      </c>
+      <c r="L3">
+        <v>2</v>
+      </c>
+      <c r="M3">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="N3">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="P3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>0.382653061224489</v>
+      </c>
+      <c r="S3">
+        <v>0.12704081632653</v>
+      </c>
+      <c r="T3">
+        <v>2</v>
+      </c>
+      <c r="U3">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="V3">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -981,8 +1089,50 @@
       <c r="F4">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0.35111623519547203</v>
+      </c>
+      <c r="K4">
+        <v>0.13756943716591499</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="N4">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="P4" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0.35111623519547203</v>
+      </c>
+      <c r="S4">
+        <v>0.13808301016664901</v>
+      </c>
+      <c r="T4">
+        <v>2</v>
+      </c>
+      <c r="U4">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="V4">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -1001,8 +1151,50 @@
       <c r="F5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0.34948979591836699</v>
+      </c>
+      <c r="K5">
+        <v>0.141765306122448</v>
+      </c>
+      <c r="L5">
+        <v>2</v>
+      </c>
+      <c r="M5">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="N5">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="P5" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0.34183673469387699</v>
+      </c>
+      <c r="S5">
+        <v>0.13932142857142801</v>
+      </c>
+      <c r="T5">
+        <v>2</v>
+      </c>
+      <c r="U5">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="V5">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1021,8 +1213,50 @@
       <c r="F6">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.59523809523809501</v>
+      </c>
+      <c r="K6">
+        <v>0.21441326530612201</v>
+      </c>
+      <c r="L6">
+        <v>3</v>
+      </c>
+      <c r="M6">
+        <v>0.21276595744680801</v>
+      </c>
+      <c r="N6">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="P6" t="s">
+        <v>9</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0.51020408163265296</v>
+      </c>
+      <c r="S6">
+        <v>0.20778061224489699</v>
+      </c>
+      <c r="T6">
+        <v>3</v>
+      </c>
+      <c r="U6">
+        <v>0.21276595744680801</v>
+      </c>
+      <c r="V6">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -1041,8 +1275,50 @@
       <c r="F7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0.75818789054083102</v>
+      </c>
+      <c r="K7">
+        <v>0.27149051928463602</v>
+      </c>
+      <c r="L7">
+        <v>4</v>
+      </c>
+      <c r="M7">
+        <v>0.28368794326241098</v>
+      </c>
+      <c r="N7">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="P7" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>0.75818789054083102</v>
+      </c>
+      <c r="S7">
+        <v>0.27474547511312197</v>
+      </c>
+      <c r="T7">
+        <v>4</v>
+      </c>
+      <c r="U7">
+        <v>0.28368794326241098</v>
+      </c>
+      <c r="V7">
+        <v>0.28399999999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -1061,8 +1337,50 @@
       <c r="F8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8">
+        <v>0.20333937776602001</v>
+      </c>
+      <c r="J8">
+        <v>0.79771830485985395</v>
+      </c>
+      <c r="K8">
+        <v>0.47639955502370102</v>
+      </c>
+      <c r="L8">
+        <v>7</v>
+      </c>
+      <c r="M8">
+        <v>0.49645390070921902</v>
+      </c>
+      <c r="N8">
+        <v>0.496</v>
+      </c>
+      <c r="P8" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q8">
+        <v>0.19893899204244</v>
+      </c>
+      <c r="R8">
+        <v>0.80732303947678796</v>
+      </c>
+      <c r="S8">
+        <v>0.47632356393335501</v>
+      </c>
+      <c r="T8">
+        <v>7</v>
+      </c>
+      <c r="U8">
+        <v>0.49645390070921902</v>
+      </c>
+      <c r="V8">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1081,8 +1399,50 @@
       <c r="F9">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H9" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>6.3775510204081606E-2</v>
+      </c>
+      <c r="J9">
+        <v>1.06153175555936</v>
+      </c>
+      <c r="K9">
+        <v>0.48554636140170299</v>
+      </c>
+      <c r="L9">
+        <v>7</v>
+      </c>
+      <c r="M9">
+        <v>0.49645390070921902</v>
+      </c>
+      <c r="N9">
+        <v>0.496</v>
+      </c>
+      <c r="P9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9">
+        <v>7.0028011204481794E-2</v>
+      </c>
+      <c r="R9">
+        <v>1.06363974161093</v>
+      </c>
+      <c r="S9">
+        <v>0.47851140456182401</v>
+      </c>
+      <c r="T9">
+        <v>7</v>
+      </c>
+      <c r="U9">
+        <v>0.49645390070921902</v>
+      </c>
+      <c r="V9">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1101,8 +1461,50 @@
       <c r="F10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H10" t="s">
+        <v>13</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>4.59183673469387</v>
+      </c>
+      <c r="K10">
+        <v>1.47397959183673</v>
+      </c>
+      <c r="L10">
+        <v>9</v>
+      </c>
+      <c r="M10">
+        <v>0.63829787234042501</v>
+      </c>
+      <c r="N10">
+        <v>0.63800000000000001</v>
+      </c>
+      <c r="P10" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>4.59183673469387</v>
+      </c>
+      <c r="S10">
+        <v>1.5290816326530601</v>
+      </c>
+      <c r="T10">
+        <v>9</v>
+      </c>
+      <c r="U10">
+        <v>0.63829787234042501</v>
+      </c>
+      <c r="V10">
+        <v>0.63800000000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1121,8 +1523,50 @@
       <c r="F11">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H11" t="s">
+        <v>14</v>
+      </c>
+      <c r="I11">
+        <v>0.33478535645027202</v>
+      </c>
+      <c r="J11">
+        <v>3.7413473860240001</v>
+      </c>
+      <c r="K11">
+        <v>1.7916410428640299</v>
+      </c>
+      <c r="L11">
+        <v>21</v>
+      </c>
+      <c r="M11">
+        <v>1.48936170212765</v>
+      </c>
+      <c r="N11">
+        <v>1.4890000000000001</v>
+      </c>
+      <c r="P11" t="s">
+        <v>14</v>
+      </c>
+      <c r="Q11">
+        <v>0.33840138619550297</v>
+      </c>
+      <c r="R11">
+        <v>3.88913864538489</v>
+      </c>
+      <c r="S11">
+        <v>1.78246557780621</v>
+      </c>
+      <c r="T11">
+        <v>21</v>
+      </c>
+      <c r="U11">
+        <v>1.48936170212765</v>
+      </c>
+      <c r="V11">
+        <v>1.4890000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1141,8 +1585,50 @@
       <c r="F12">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H12" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>4.3424773755655997</v>
+      </c>
+      <c r="K12">
+        <v>1.60031512605042</v>
+      </c>
+      <c r="L12">
+        <v>22</v>
+      </c>
+      <c r="M12">
+        <v>1.56028368794326</v>
+      </c>
+      <c r="N12">
+        <v>1.56</v>
+      </c>
+      <c r="P12" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>4.2663219133807297</v>
+      </c>
+      <c r="S12">
+        <v>1.50263817065287</v>
+      </c>
+      <c r="T12">
+        <v>22</v>
+      </c>
+      <c r="U12">
+        <v>1.56028368794326</v>
+      </c>
+      <c r="V12">
+        <v>1.56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1161,8 +1647,50 @@
       <c r="F13">
         <v>25</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>5.0437014428412796</v>
+      </c>
+      <c r="K13">
+        <v>1.79630437080492</v>
+      </c>
+      <c r="L13">
+        <v>25</v>
+      </c>
+      <c r="M13">
+        <v>1.7730496453900699</v>
+      </c>
+      <c r="N13">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="P13" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>4.6165636065747</v>
+      </c>
+      <c r="S13">
+        <v>1.72769806035621</v>
+      </c>
+      <c r="T13">
+        <v>25</v>
+      </c>
+      <c r="U13">
+        <v>1.7730496453900699</v>
+      </c>
+      <c r="V13">
+        <v>1.7729999999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1181,8 +1709,50 @@
       <c r="F14">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H14" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14">
+        <v>0.206193588546529</v>
+      </c>
+      <c r="J14">
+        <v>4.8379967028740198</v>
+      </c>
+      <c r="K14">
+        <v>2.0580865438418501</v>
+      </c>
+      <c r="L14">
+        <v>31</v>
+      </c>
+      <c r="M14">
+        <v>2.1985815602836798</v>
+      </c>
+      <c r="N14">
+        <v>2.1989999999999998</v>
+      </c>
+      <c r="P14" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q14">
+        <v>0.206193588546529</v>
+      </c>
+      <c r="R14">
+        <v>4.7860464940693204</v>
+      </c>
+      <c r="S14">
+        <v>2.1003093050637398</v>
+      </c>
+      <c r="T14">
+        <v>31</v>
+      </c>
+      <c r="U14">
+        <v>2.1985815602836798</v>
+      </c>
+      <c r="V14">
+        <v>2.1989999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1201,8 +1771,50 @@
       <c r="F15">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I15">
+        <v>1.3220960909376001</v>
+      </c>
+      <c r="J15">
+        <v>6.9087963366911698</v>
+      </c>
+      <c r="K15">
+        <v>3.92485590241255</v>
+      </c>
+      <c r="L15">
+        <v>41</v>
+      </c>
+      <c r="M15">
+        <v>2.9078014184397101</v>
+      </c>
+      <c r="N15">
+        <v>2.9079999999999999</v>
+      </c>
+      <c r="P15" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15">
+        <v>1.6211900536544901</v>
+      </c>
+      <c r="R15">
+        <v>7.2137843450928703</v>
+      </c>
+      <c r="S15">
+        <v>3.98827260438014</v>
+      </c>
+      <c r="T15">
+        <v>41</v>
+      </c>
+      <c r="U15">
+        <v>2.9078014184397101</v>
+      </c>
+      <c r="V15">
+        <v>2.9079999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1221,8 +1833,50 @@
       <c r="F16">
         <v>48</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16">
+        <v>1.14831236175745</v>
+      </c>
+      <c r="J16">
+        <v>7.5974264584161704</v>
+      </c>
+      <c r="K16">
+        <v>3.7507350074423398</v>
+      </c>
+      <c r="L16">
+        <v>48</v>
+      </c>
+      <c r="M16">
+        <v>3.40425531914893</v>
+      </c>
+      <c r="N16">
+        <v>3.4039999999999999</v>
+      </c>
+      <c r="P16" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q16">
+        <v>1.0150515187990401</v>
+      </c>
+      <c r="R16">
+        <v>7.8064851659661603</v>
+      </c>
+      <c r="S16">
+        <v>3.7136072173141299</v>
+      </c>
+      <c r="T16">
+        <v>48</v>
+      </c>
+      <c r="U16">
+        <v>3.40425531914893</v>
+      </c>
+      <c r="V16">
+        <v>3.4039999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1241,8 +1895,50 @@
       <c r="F17">
         <v>51</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H17" t="s">
+        <v>20</v>
+      </c>
+      <c r="I17">
+        <v>1.71382485514459</v>
+      </c>
+      <c r="J17">
+        <v>6.2023397343440996</v>
+      </c>
+      <c r="K17">
+        <v>3.7213867741167599</v>
+      </c>
+      <c r="L17">
+        <v>51</v>
+      </c>
+      <c r="M17">
+        <v>3.6170212765957399</v>
+      </c>
+      <c r="N17">
+        <v>3.617</v>
+      </c>
+      <c r="P17" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q17">
+        <v>1.67743566034342</v>
+      </c>
+      <c r="R17">
+        <v>6.2894924457515504</v>
+      </c>
+      <c r="S17">
+        <v>3.6863495615299602</v>
+      </c>
+      <c r="T17">
+        <v>51</v>
+      </c>
+      <c r="U17">
+        <v>3.6170212765957399</v>
+      </c>
+      <c r="V17">
+        <v>3.617</v>
+      </c>
+    </row>
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>21</v>
       </c>
@@ -1261,8 +1957,50 @@
       <c r="F18">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18">
+        <v>3.19964329242414</v>
+      </c>
+      <c r="J18">
+        <v>9.2235615178518504</v>
+      </c>
+      <c r="K18">
+        <v>5.9080610984080097</v>
+      </c>
+      <c r="L18">
+        <v>73</v>
+      </c>
+      <c r="M18">
+        <v>5.1773049645390001</v>
+      </c>
+      <c r="N18">
+        <v>5.1769999999999996</v>
+      </c>
+      <c r="P18" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q18">
+        <v>3.3241672192356901</v>
+      </c>
+      <c r="R18">
+        <v>9.1817512299597297</v>
+      </c>
+      <c r="S18">
+        <v>5.9941779272999396</v>
+      </c>
+      <c r="T18">
+        <v>73</v>
+      </c>
+      <c r="U18">
+        <v>5.1773049645390001</v>
+      </c>
+      <c r="V18">
+        <v>5.1769999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1281,13 +2019,55 @@
       <c r="F19">
         <v>79</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H19" t="s">
+        <v>22</v>
+      </c>
+      <c r="I19">
+        <v>3.4490019295543499</v>
+      </c>
+      <c r="J19">
+        <v>7.9059980799206597</v>
+      </c>
+      <c r="K19">
+        <v>5.5312466339320601</v>
+      </c>
+      <c r="L19">
+        <v>79</v>
+      </c>
+      <c r="M19">
+        <v>5.60283687943262</v>
+      </c>
+      <c r="N19">
+        <v>5.6029999999999998</v>
+      </c>
+      <c r="P19" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q19">
+        <v>3.5700916655274599</v>
+      </c>
+      <c r="R19">
+        <v>8.0988022070530796</v>
+      </c>
+      <c r="S19">
+        <v>5.5137077609761898</v>
+      </c>
+      <c r="T19">
+        <v>79</v>
+      </c>
+      <c r="U19">
+        <v>5.60283687943262</v>
+      </c>
+      <c r="V19">
+        <v>5.6029999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1306,8 +2086,50 @@
       <c r="F22" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H22" t="s">
+        <v>0</v>
+      </c>
+      <c r="I22" t="s">
+        <v>1</v>
+      </c>
+      <c r="J22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>3</v>
+      </c>
+      <c r="L22" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" t="s">
+        <v>5</v>
+      </c>
+      <c r="N22" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" t="s">
+        <v>3</v>
+      </c>
+      <c r="T22" t="s">
+        <v>4</v>
+      </c>
+      <c r="U22" t="s">
+        <v>5</v>
+      </c>
+      <c r="V22" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>11</v>
       </c>
@@ -1326,8 +2148,50 @@
       <c r="F23">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0.223214285714285</v>
+      </c>
+      <c r="K23">
+        <v>7.1354166666666594E-2</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>7.09219858156028E-2</v>
+      </c>
+      <c r="N23">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="P23" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0.21865889212827899</v>
+      </c>
+      <c r="S23">
+        <v>7.0408163265306106E-2</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>7.09219858156028E-2</v>
+      </c>
+      <c r="V23">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>25</v>
       </c>
@@ -1346,8 +2210,50 @@
       <c r="F24">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H24" t="s">
+        <v>11</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0.21865889212827899</v>
+      </c>
+      <c r="K24">
+        <v>7.1428571428571397E-2</v>
+      </c>
+      <c r="L24">
+        <v>1</v>
+      </c>
+      <c r="M24">
+        <v>7.09219858156028E-2</v>
+      </c>
+      <c r="N24">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="P24" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0.223214285714285</v>
+      </c>
+      <c r="S24">
+        <v>7.5520833333333301E-2</v>
+      </c>
+      <c r="T24">
+        <v>1</v>
+      </c>
+      <c r="U24">
+        <v>7.09219858156028E-2</v>
+      </c>
+      <c r="V24">
+        <v>7.0999999999999994E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1366,8 +2272,50 @@
       <c r="F25">
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0.33068783068782998</v>
+      </c>
+      <c r="K25">
+        <v>0.13029100529100501</v>
+      </c>
+      <c r="L25">
+        <v>2</v>
+      </c>
+      <c r="M25">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="N25">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="P25" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>0.33068783068782998</v>
+      </c>
+      <c r="S25">
+        <v>0.136044973544973</v>
+      </c>
+      <c r="T25">
+        <v>2</v>
+      </c>
+      <c r="U25">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="V25">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>13</v>
       </c>
@@ -1386,8 +2334,50 @@
       <c r="F26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H26" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0.43243243243243201</v>
+      </c>
+      <c r="K26">
+        <v>0.165938223938223</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+      <c r="M26">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="N26">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="P26" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0.43243243243243201</v>
+      </c>
+      <c r="S26">
+        <v>0.16741505791505701</v>
+      </c>
+      <c r="T26">
+        <v>2</v>
+      </c>
+      <c r="U26">
+        <v>0.14184397163120499</v>
+      </c>
+      <c r="V26">
+        <v>0.14199999999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1406,8 +2396,50 @@
       <c r="F27">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H27" t="s">
+        <v>7</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>0.44297523129481398</v>
+      </c>
+      <c r="K27">
+        <v>0.20946686171935799</v>
+      </c>
+      <c r="L27">
+        <v>3</v>
+      </c>
+      <c r="M27">
+        <v>0.21276595744680801</v>
+      </c>
+      <c r="N27">
+        <v>0.21299999999999999</v>
+      </c>
+      <c r="P27" t="s">
+        <v>7</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0.49623851566969202</v>
+      </c>
+      <c r="S27">
+        <v>0.21241944599521601</v>
+      </c>
+      <c r="T27">
+        <v>3</v>
+      </c>
+      <c r="U27">
+        <v>0.21276595744680801</v>
+      </c>
+      <c r="V27">
+        <v>0.21299999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>18</v>
       </c>
@@ -1426,8 +2458,50 @@
       <c r="F28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H28" t="s">
+        <v>18</v>
+      </c>
+      <c r="I28">
+        <v>6.6137566137566106E-2</v>
+      </c>
+      <c r="J28">
+        <v>0.66137566137566095</v>
+      </c>
+      <c r="K28">
+        <v>0.33604497354497298</v>
+      </c>
+      <c r="L28">
+        <v>5</v>
+      </c>
+      <c r="M28">
+        <v>0.35460992907801397</v>
+      </c>
+      <c r="N28">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="P28" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q28">
+        <v>6.6137566137566106E-2</v>
+      </c>
+      <c r="R28">
+        <v>0.66302910052909803</v>
+      </c>
+      <c r="S28">
+        <v>0.31990740740740697</v>
+      </c>
+      <c r="T28">
+        <v>5</v>
+      </c>
+      <c r="U28">
+        <v>0.35460992907801397</v>
+      </c>
+      <c r="V28">
+        <v>0.35499999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>19</v>
       </c>
@@ -1446,8 +2520,50 @@
       <c r="F29">
         <v>7</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H29" t="s">
+        <v>19</v>
+      </c>
+      <c r="I29">
+        <v>7.4404761904761793E-2</v>
+      </c>
+      <c r="J29">
+        <v>1.0704910348060399</v>
+      </c>
+      <c r="K29">
+        <v>0.51489034158235303</v>
+      </c>
+      <c r="L29">
+        <v>7</v>
+      </c>
+      <c r="M29">
+        <v>0.49645390070921902</v>
+      </c>
+      <c r="N29">
+        <v>0.496</v>
+      </c>
+      <c r="P29" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q29">
+        <v>0.13352301088150101</v>
+      </c>
+      <c r="R29">
+        <v>1.1253176800525999</v>
+      </c>
+      <c r="S29">
+        <v>0.50355063728617799</v>
+      </c>
+      <c r="T29">
+        <v>7</v>
+      </c>
+      <c r="U29">
+        <v>0.49645390070921902</v>
+      </c>
+      <c r="V29">
+        <v>0.496</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>12</v>
       </c>
@@ -1466,8 +2582,50 @@
       <c r="F30">
         <v>15</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H30" t="s">
+        <v>12</v>
+      </c>
+      <c r="I30">
+        <v>0.307255186996167</v>
+      </c>
+      <c r="J30">
+        <v>2.41091893001532</v>
+      </c>
+      <c r="K30">
+        <v>1.2733966532993299</v>
+      </c>
+      <c r="L30">
+        <v>15</v>
+      </c>
+      <c r="M30">
+        <v>1.0638297872340401</v>
+      </c>
+      <c r="N30">
+        <v>1.0640000000000001</v>
+      </c>
+      <c r="P30" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q30">
+        <v>0.39820194860776298</v>
+      </c>
+      <c r="R30">
+        <v>2.3406238548426299</v>
+      </c>
+      <c r="S30">
+        <v>1.29446527790629</v>
+      </c>
+      <c r="T30">
+        <v>15</v>
+      </c>
+      <c r="U30">
+        <v>1.0638297872340401</v>
+      </c>
+      <c r="V30">
+        <v>1.0640000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1486,8 +2644,50 @@
       <c r="F31">
         <v>18</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H31" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31">
+        <v>0.573700701534269</v>
+      </c>
+      <c r="J31">
+        <v>2.77044178031564</v>
+      </c>
+      <c r="K31">
+        <v>1.52414373401463</v>
+      </c>
+      <c r="L31">
+        <v>18</v>
+      </c>
+      <c r="M31">
+        <v>1.27659574468085</v>
+      </c>
+      <c r="N31">
+        <v>1.2769999999999999</v>
+      </c>
+      <c r="P31" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q31">
+        <v>0.57649840668643104</v>
+      </c>
+      <c r="R31">
+        <v>2.62400961018818</v>
+      </c>
+      <c r="S31">
+        <v>1.4825812669153999</v>
+      </c>
+      <c r="T31">
+        <v>18</v>
+      </c>
+      <c r="U31">
+        <v>1.27659574468085</v>
+      </c>
+      <c r="V31">
+        <v>1.2769999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>16</v>
       </c>
@@ -1506,8 +2706,50 @@
       <c r="F32">
         <v>23</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H32" t="s">
+        <v>16</v>
+      </c>
+      <c r="I32">
+        <v>0.54447938504542204</v>
+      </c>
+      <c r="J32">
+        <v>3.3228799328630201</v>
+      </c>
+      <c r="K32">
+        <v>1.6407184249508699</v>
+      </c>
+      <c r="L32">
+        <v>23</v>
+      </c>
+      <c r="M32">
+        <v>1.6312056737588601</v>
+      </c>
+      <c r="N32">
+        <v>1.631</v>
+      </c>
+      <c r="P32" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q32">
+        <v>0.49361720279606303</v>
+      </c>
+      <c r="R32">
+        <v>3.23136872507509</v>
+      </c>
+      <c r="S32">
+        <v>1.6552033888883999</v>
+      </c>
+      <c r="T32">
+        <v>23</v>
+      </c>
+      <c r="U32">
+        <v>1.6312056737588601</v>
+      </c>
+      <c r="V32">
+        <v>1.631</v>
+      </c>
+    </row>
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>17</v>
       </c>
@@ -1526,8 +2768,50 @@
       <c r="F33">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H33" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33">
+        <v>0.70968638928991801</v>
+      </c>
+      <c r="J33">
+        <v>3.2153489091199701</v>
+      </c>
+      <c r="K33">
+        <v>1.7415609579311</v>
+      </c>
+      <c r="L33">
+        <v>25</v>
+      </c>
+      <c r="M33">
+        <v>1.7730496453900699</v>
+      </c>
+      <c r="N33">
+        <v>1.7729999999999999</v>
+      </c>
+      <c r="P33" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q33">
+        <v>0.76687889908645201</v>
+      </c>
+      <c r="R33">
+        <v>3.08591049146108</v>
+      </c>
+      <c r="S33">
+        <v>1.7245275108624101</v>
+      </c>
+      <c r="T33">
+        <v>25</v>
+      </c>
+      <c r="U33">
+        <v>1.7730496453900699</v>
+      </c>
+      <c r="V33">
+        <v>1.7729999999999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>23</v>
       </c>
@@ -1546,8 +2830,50 @@
       <c r="F34">
         <v>30</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H34" t="s">
+        <v>23</v>
+      </c>
+      <c r="I34">
+        <v>1.33469975085721</v>
+      </c>
+      <c r="J34">
+        <v>3.7376595225309002</v>
+      </c>
+      <c r="K34">
+        <v>2.3832713575301598</v>
+      </c>
+      <c r="L34">
+        <v>30</v>
+      </c>
+      <c r="M34">
+        <v>2.1276595744680802</v>
+      </c>
+      <c r="N34">
+        <v>2.1280000000000001</v>
+      </c>
+      <c r="P34" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q34">
+        <v>1.3342980803806901</v>
+      </c>
+      <c r="R34">
+        <v>3.7686615993047501</v>
+      </c>
+      <c r="S34">
+        <v>2.38093962761985</v>
+      </c>
+      <c r="T34">
+        <v>30</v>
+      </c>
+      <c r="U34">
+        <v>2.1276595744680802</v>
+      </c>
+      <c r="V34">
+        <v>2.1280000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>20</v>
       </c>
@@ -1566,8 +2892,50 @@
       <c r="F35">
         <v>54</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="H35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <v>2.1604945062780998</v>
+      </c>
+      <c r="J35">
+        <v>5.9396779359848599</v>
+      </c>
+      <c r="K35">
+        <v>4.0211021229747903</v>
+      </c>
+      <c r="L35">
+        <v>54</v>
+      </c>
+      <c r="M35">
+        <v>3.8297872340425498</v>
+      </c>
+      <c r="N35">
+        <v>3.83</v>
+      </c>
+      <c r="P35" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q35">
+        <v>2.2111490021366902</v>
+      </c>
+      <c r="R35">
+        <v>6.0536529344490999</v>
+      </c>
+      <c r="S35">
+        <v>4.0033764800703899</v>
+      </c>
+      <c r="T35">
+        <v>54</v>
+      </c>
+      <c r="U35">
+        <v>3.8297872340425498</v>
+      </c>
+      <c r="V35">
+        <v>3.83</v>
+      </c>
+    </row>
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>22</v>
       </c>
@@ -1585,6 +2953,48 @@
       </c>
       <c r="F36">
         <v>55</v>
+      </c>
+      <c r="H36" t="s">
+        <v>22</v>
+      </c>
+      <c r="I36">
+        <v>1.88270559613873</v>
+      </c>
+      <c r="J36">
+        <v>6.6797482910075097</v>
+      </c>
+      <c r="K36">
+        <v>4.0516115666300401</v>
+      </c>
+      <c r="L36">
+        <v>55</v>
+      </c>
+      <c r="M36">
+        <v>3.9007092198581499</v>
+      </c>
+      <c r="N36">
+        <v>3.9009999999999998</v>
+      </c>
+      <c r="P36" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q36">
+        <v>1.9402700463559699</v>
+      </c>
+      <c r="R36">
+        <v>6.5462497359760699</v>
+      </c>
+      <c r="S36">
+        <v>4.07986996747786</v>
+      </c>
+      <c r="T36">
+        <v>55</v>
+      </c>
+      <c r="U36">
+        <v>3.9007092198581499</v>
+      </c>
+      <c r="V36">
+        <v>3.9009999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>